<commit_message>
changing USA to india
</commit_message>
<xml_diff>
--- a/csvfiles/Holiday Calendar 2022_V 1.4.xlsx
+++ b/csvfiles/Holiday Calendar 2022_V 1.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mphasis-my.sharepoint.com/personal/mary_mammen_mphasis_com/Documents/DATA BACKUP_Feb 2020/mary Smitha Databackup/Backup/user data 4331/Back-up data_Smita_July 2019/Holiday Calendar/2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eytham.kishore\Documents\testrepo\Testrepo\csvfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6929DBCF-7E9C-4C51-95B1-82338028454E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A098D2FD-5DC2-435C-9F40-D400BC8175BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="4" activeTab="6" xr2:uid="{7CB9B53B-FCCC-41BF-A5C9-0C70CDEA78CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{7CB9B53B-FCCC-41BF-A5C9-0C70CDEA78CC}"/>
   </bookViews>
   <sheets>
     <sheet name="India Holidays 2022" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="379">
   <si>
     <t>Karnataka</t>
   </si>
@@ -1314,6 +1314,9 @@
   </si>
   <si>
     <t>Christmas Day (in lieu)</t>
+  </si>
+  <si>
+    <t>INDIA</t>
   </si>
 </sst>
 </file>
@@ -2983,6 +2986,15 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2992,6 +3004,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3013,20 +3031,32 @@
     <xf numFmtId="164" fontId="11" fillId="9" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="10" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="16" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3061,48 +3091,39 @@
     <xf numFmtId="164" fontId="18" fillId="10" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="15" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="15" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="10" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="16" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="32" fillId="10" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="16" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="15" borderId="60" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="16" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="15" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3110,24 +3131,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="15" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="10" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="11" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6447,28 +6450,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="198" t="s">
         <v>236</v>
       </c>
       <c r="B1" s="28"/>
       <c r="P1" s="29"/>
-      <c r="Z1" s="195" t="s">
+      <c r="Z1" s="200" t="s">
         <v>93</v>
       </c>
-      <c r="AA1" s="196"/>
-      <c r="AB1" s="196"/>
-      <c r="AC1" s="196"/>
-      <c r="AD1" s="196"/>
-      <c r="AE1" s="197"/>
-      <c r="AF1" s="198" t="s">
+      <c r="AA1" s="201"/>
+      <c r="AB1" s="201"/>
+      <c r="AC1" s="201"/>
+      <c r="AD1" s="201"/>
+      <c r="AE1" s="202"/>
+      <c r="AF1" s="203" t="s">
         <v>94</v>
       </c>
-      <c r="AG1" s="198"/>
-      <c r="AH1" s="198"/>
-      <c r="AI1" s="199"/>
+      <c r="AG1" s="203"/>
+      <c r="AH1" s="203"/>
+      <c r="AI1" s="204"/>
     </row>
     <row r="2" spans="1:35" ht="64.5" thickBot="1">
-      <c r="A2" s="194"/>
+      <c r="A2" s="199"/>
       <c r="B2" s="30" t="s">
         <v>95</v>
       </c>
@@ -6573,7 +6576,7 @@
       </c>
     </row>
     <row r="3" spans="1:35">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="193" t="s">
         <v>129</v>
       </c>
       <c r="B3" s="38">
@@ -6677,7 +6680,7 @@
       </c>
     </row>
     <row r="4" spans="1:35">
-      <c r="A4" s="191"/>
+      <c r="A4" s="194"/>
       <c r="B4" s="41">
         <f t="shared" ref="B4:D4" si="0">B3</f>
         <v>44564</v>
@@ -6812,7 +6815,7 @@
       </c>
     </row>
     <row r="5" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A5" s="191"/>
+      <c r="A5" s="194"/>
       <c r="B5" s="43" t="s">
         <v>250</v>
       </c>
@@ -6914,7 +6917,7 @@
       </c>
     </row>
     <row r="6" spans="1:35">
-      <c r="A6" s="191"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="37">
         <v>44578</v>
       </c>
@@ -6975,7 +6978,7 @@
       </c>
     </row>
     <row r="7" spans="1:35">
-      <c r="A7" s="191"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="40">
         <f>B6</f>
         <v>44578</v>
@@ -7053,7 +7056,7 @@
       </c>
     </row>
     <row r="8" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A8" s="191"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="43" t="s">
         <v>130</v>
       </c>
@@ -7114,7 +7117,7 @@
       </c>
     </row>
     <row r="9" spans="1:35">
-      <c r="A9" s="191"/>
+      <c r="A9" s="194"/>
       <c r="B9" s="54"/>
       <c r="E9" s="45"/>
       <c r="F9" s="131"/>
@@ -7138,7 +7141,7 @@
       </c>
     </row>
     <row r="10" spans="1:35">
-      <c r="A10" s="191"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="54"/>
       <c r="E10" s="45"/>
       <c r="F10" s="131"/>
@@ -7165,7 +7168,7 @@
       </c>
     </row>
     <row r="11" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A11" s="191"/>
+      <c r="A11" s="194"/>
       <c r="B11" s="54"/>
       <c r="E11" s="45"/>
       <c r="F11" s="131"/>
@@ -7189,7 +7192,7 @@
       </c>
     </row>
     <row r="12" spans="1:35">
-      <c r="A12" s="191"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="54"/>
       <c r="E12" s="45"/>
       <c r="F12" s="131"/>
@@ -7203,7 +7206,7 @@
       <c r="AE12" s="56"/>
     </row>
     <row r="13" spans="1:35">
-      <c r="A13" s="191"/>
+      <c r="A13" s="194"/>
       <c r="B13" s="54"/>
       <c r="E13" s="45"/>
       <c r="F13" s="131"/>
@@ -7217,7 +7220,7 @@
       <c r="AE13" s="56"/>
     </row>
     <row r="14" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A14" s="192"/>
+      <c r="A14" s="195"/>
       <c r="B14" s="57"/>
       <c r="C14" s="58"/>
       <c r="D14" s="58"/>
@@ -7254,7 +7257,7 @@
       <c r="AI14" s="58"/>
     </row>
     <row r="15" spans="1:35">
-      <c r="A15" s="200" t="s">
+      <c r="A15" s="190" t="s">
         <v>137</v>
       </c>
       <c r="B15" s="37">
@@ -7308,7 +7311,7 @@
       </c>
     </row>
     <row r="16" spans="1:35">
-      <c r="A16" s="201"/>
+      <c r="A16" s="191"/>
       <c r="B16" s="40">
         <f>B15</f>
         <v>44613</v>
@@ -7372,7 +7375,7 @@
       </c>
     </row>
     <row r="17" spans="1:35" ht="77.25" thickBot="1">
-      <c r="A17" s="201"/>
+      <c r="A17" s="191"/>
       <c r="B17" s="43" t="s">
         <v>140</v>
       </c>
@@ -7424,7 +7427,7 @@
       </c>
     </row>
     <row r="18" spans="1:35">
-      <c r="A18" s="201"/>
+      <c r="A18" s="191"/>
       <c r="B18" s="54"/>
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
@@ -7448,7 +7451,7 @@
       <c r="AI18" s="56"/>
     </row>
     <row r="19" spans="1:35">
-      <c r="A19" s="201"/>
+      <c r="A19" s="191"/>
       <c r="B19" s="54"/>
       <c r="C19" s="45"/>
       <c r="D19" s="45"/>
@@ -7476,7 +7479,7 @@
       <c r="AI19" s="56"/>
     </row>
     <row r="20" spans="1:35" ht="51.75" thickBot="1">
-      <c r="A20" s="202"/>
+      <c r="A20" s="192"/>
       <c r="B20" s="57"/>
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
@@ -7516,7 +7519,7 @@
       <c r="AI20" s="62"/>
     </row>
     <row r="21" spans="1:35">
-      <c r="A21" s="190" t="s">
+      <c r="A21" s="193" t="s">
         <v>148</v>
       </c>
       <c r="B21" s="54"/>
@@ -7573,7 +7576,7 @@
       <c r="AI21" s="75"/>
     </row>
     <row r="22" spans="1:35">
-      <c r="A22" s="191"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="54"/>
       <c r="C22" s="49">
         <f>C21</f>
@@ -7629,7 +7632,7 @@
       <c r="AI22" s="56"/>
     </row>
     <row r="23" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A23" s="191"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="54"/>
       <c r="C23" s="77" t="s">
         <v>239</v>
@@ -7676,7 +7679,7 @@
       <c r="AI23" s="56"/>
     </row>
     <row r="24" spans="1:35">
-      <c r="A24" s="191"/>
+      <c r="A24" s="194"/>
       <c r="B24" s="54"/>
       <c r="E24" s="45"/>
       <c r="H24" s="47"/>
@@ -7689,7 +7692,7 @@
       <c r="AI24" s="56"/>
     </row>
     <row r="25" spans="1:35">
-      <c r="A25" s="191"/>
+      <c r="A25" s="194"/>
       <c r="B25" s="54"/>
       <c r="E25" s="45"/>
       <c r="H25" s="47"/>
@@ -7703,7 +7706,7 @@
       <c r="AI25" s="56"/>
     </row>
     <row r="26" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A26" s="192"/>
+      <c r="A26" s="195"/>
       <c r="B26" s="57"/>
       <c r="C26" s="59"/>
       <c r="D26" s="59"/>
@@ -7741,7 +7744,7 @@
       <c r="AI26" s="62"/>
     </row>
     <row r="27" spans="1:35">
-      <c r="A27" s="200" t="s">
+      <c r="A27" s="190" t="s">
         <v>154</v>
       </c>
       <c r="B27" s="37">
@@ -7840,7 +7843,7 @@
       </c>
     </row>
     <row r="28" spans="1:35">
-      <c r="A28" s="201"/>
+      <c r="A28" s="191"/>
       <c r="B28" s="40">
         <f>B27</f>
         <v>44666</v>
@@ -7967,7 +7970,7 @@
       </c>
     </row>
     <row r="29" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A29" s="201"/>
+      <c r="A29" s="191"/>
       <c r="B29" s="43" t="s">
         <v>46</v>
       </c>
@@ -8066,7 +8069,7 @@
       </c>
     </row>
     <row r="30" spans="1:35">
-      <c r="A30" s="201"/>
+      <c r="A30" s="191"/>
       <c r="B30" s="54"/>
       <c r="C30" s="37">
         <v>44666</v>
@@ -8145,7 +8148,7 @@
       </c>
     </row>
     <row r="31" spans="1:35">
-      <c r="A31" s="201"/>
+      <c r="A31" s="191"/>
       <c r="B31" s="54"/>
       <c r="C31" s="40">
         <f t="shared" ref="C31:D31" si="34">C30</f>
@@ -8247,7 +8250,7 @@
       </c>
     </row>
     <row r="32" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A32" s="201"/>
+      <c r="A32" s="191"/>
       <c r="B32" s="54"/>
       <c r="C32" s="43" t="s">
         <v>156</v>
@@ -8325,7 +8328,7 @@
       </c>
     </row>
     <row r="33" spans="1:35">
-      <c r="A33" s="201"/>
+      <c r="A33" s="191"/>
       <c r="B33" s="54"/>
       <c r="D33" s="37">
         <v>44666</v>
@@ -8383,7 +8386,7 @@
       </c>
     </row>
     <row r="34" spans="1:35">
-      <c r="A34" s="201"/>
+      <c r="A34" s="191"/>
       <c r="B34" s="54"/>
       <c r="D34" s="40">
         <f t="shared" ref="D34" si="44">D33</f>
@@ -8453,7 +8456,7 @@
       </c>
     </row>
     <row r="35" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A35" s="201"/>
+      <c r="A35" s="191"/>
       <c r="B35" s="54"/>
       <c r="D35" s="43" t="s">
         <v>46</v>
@@ -8511,7 +8514,7 @@
       </c>
     </row>
     <row r="36" spans="1:35">
-      <c r="A36" s="201"/>
+      <c r="A36" s="191"/>
       <c r="B36" s="54"/>
       <c r="D36" s="47"/>
       <c r="E36" s="45"/>
@@ -8524,7 +8527,7 @@
       <c r="AE36" s="56"/>
     </row>
     <row r="37" spans="1:35">
-      <c r="A37" s="201"/>
+      <c r="A37" s="191"/>
       <c r="B37" s="54"/>
       <c r="D37" s="47"/>
       <c r="E37" s="45"/>
@@ -8536,7 +8539,7 @@
       <c r="AE37" s="56"/>
     </row>
     <row r="38" spans="1:35">
-      <c r="A38" s="201"/>
+      <c r="A38" s="191"/>
       <c r="B38" s="54"/>
       <c r="D38" s="47"/>
       <c r="E38" s="45"/>
@@ -8548,7 +8551,7 @@
       <c r="AE38" s="56"/>
     </row>
     <row r="39" spans="1:35">
-      <c r="A39" s="201"/>
+      <c r="A39" s="191"/>
       <c r="B39" s="54"/>
       <c r="D39" s="47"/>
       <c r="E39" s="45"/>
@@ -8560,7 +8563,7 @@
       <c r="AE39" s="56"/>
     </row>
     <row r="40" spans="1:35">
-      <c r="A40" s="201"/>
+      <c r="A40" s="191"/>
       <c r="B40" s="54"/>
       <c r="E40" s="45"/>
       <c r="H40" s="47"/>
@@ -8571,7 +8574,7 @@
       <c r="AE40" s="56"/>
     </row>
     <row r="41" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A41" s="202"/>
+      <c r="A41" s="192"/>
       <c r="B41" s="54"/>
       <c r="C41" s="58"/>
       <c r="D41" s="62"/>
@@ -8606,7 +8609,7 @@
       <c r="AI41" s="58"/>
     </row>
     <row r="42" spans="1:35">
-      <c r="A42" s="203" t="s">
+      <c r="A42" s="196" t="s">
         <v>159</v>
       </c>
       <c r="B42" s="88">
@@ -8695,7 +8698,7 @@
       <c r="AI42" s="75"/>
     </row>
     <row r="43" spans="1:35">
-      <c r="A43" s="204"/>
+      <c r="A43" s="197"/>
       <c r="B43" s="90">
         <f>B42</f>
         <v>44711</v>
@@ -8800,7 +8803,7 @@
       <c r="AI43" s="56"/>
     </row>
     <row r="44" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A44" s="204"/>
+      <c r="A44" s="197"/>
       <c r="B44" s="92" t="s">
         <v>160</v>
       </c>
@@ -8881,7 +8884,7 @@
       <c r="AI44" s="56"/>
     </row>
     <row r="45" spans="1:35">
-      <c r="A45" s="191"/>
+      <c r="A45" s="194"/>
       <c r="B45" s="54"/>
       <c r="C45" s="45"/>
       <c r="D45" s="131"/>
@@ -8921,7 +8924,7 @@
       <c r="AI45" s="56"/>
     </row>
     <row r="46" spans="1:35">
-      <c r="A46" s="191"/>
+      <c r="A46" s="194"/>
       <c r="B46" s="54"/>
       <c r="C46" s="45"/>
       <c r="D46" s="131"/>
@@ -8970,7 +8973,7 @@
       <c r="AI46" s="56"/>
     </row>
     <row r="47" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A47" s="191"/>
+      <c r="A47" s="194"/>
       <c r="B47" s="54"/>
       <c r="C47" s="45"/>
       <c r="D47" s="131"/>
@@ -9010,7 +9013,7 @@
       <c r="AI47" s="56"/>
     </row>
     <row r="48" spans="1:35">
-      <c r="A48" s="191"/>
+      <c r="A48" s="194"/>
       <c r="B48" s="54"/>
       <c r="C48" s="45"/>
       <c r="D48" s="131"/>
@@ -9031,7 +9034,7 @@
       <c r="AI48" s="56"/>
     </row>
     <row r="49" spans="1:35">
-      <c r="A49" s="191"/>
+      <c r="A49" s="194"/>
       <c r="B49" s="54"/>
       <c r="C49" s="45"/>
       <c r="D49" s="131"/>
@@ -9055,7 +9058,7 @@
       <c r="AI49" s="56"/>
     </row>
     <row r="50" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A50" s="191"/>
+      <c r="A50" s="194"/>
       <c r="B50" s="54"/>
       <c r="C50" s="45"/>
       <c r="D50" s="131"/>
@@ -9076,7 +9079,7 @@
       <c r="AI50" s="56"/>
     </row>
     <row r="51" spans="1:35">
-      <c r="A51" s="191"/>
+      <c r="A51" s="194"/>
       <c r="B51" s="54"/>
       <c r="C51" s="45"/>
       <c r="D51" s="131"/>
@@ -9091,7 +9094,7 @@
       <c r="AI51" s="56"/>
     </row>
     <row r="52" spans="1:35">
-      <c r="A52" s="191"/>
+      <c r="A52" s="194"/>
       <c r="B52" s="54"/>
       <c r="C52" s="45"/>
       <c r="D52" s="131"/>
@@ -9107,7 +9110,7 @@
       <c r="AI52" s="56"/>
     </row>
     <row r="53" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A53" s="191"/>
+      <c r="A53" s="194"/>
       <c r="B53" s="54"/>
       <c r="C53" s="45"/>
       <c r="D53" s="131"/>
@@ -9122,7 +9125,7 @@
       <c r="AI53" s="56"/>
     </row>
     <row r="54" spans="1:35">
-      <c r="A54" s="191"/>
+      <c r="A54" s="194"/>
       <c r="B54" s="54"/>
       <c r="C54" s="45"/>
       <c r="D54" s="131"/>
@@ -9134,7 +9137,7 @@
       <c r="AI54" s="56"/>
     </row>
     <row r="55" spans="1:35">
-      <c r="A55" s="191"/>
+      <c r="A55" s="194"/>
       <c r="B55" s="54"/>
       <c r="C55" s="45"/>
       <c r="D55" s="131"/>
@@ -9146,7 +9149,7 @@
       <c r="AI55" s="56"/>
     </row>
     <row r="56" spans="1:35">
-      <c r="A56" s="191"/>
+      <c r="A56" s="194"/>
       <c r="B56" s="54"/>
       <c r="C56" s="45"/>
       <c r="D56" s="131"/>
@@ -9158,7 +9161,7 @@
       <c r="AI56" s="56"/>
     </row>
     <row r="57" spans="1:35">
-      <c r="A57" s="191"/>
+      <c r="A57" s="194"/>
       <c r="B57" s="54"/>
       <c r="C57" s="45"/>
       <c r="D57" s="131"/>
@@ -9170,7 +9173,7 @@
       <c r="AI57" s="56"/>
     </row>
     <row r="58" spans="1:35">
-      <c r="A58" s="191"/>
+      <c r="A58" s="194"/>
       <c r="B58" s="54"/>
       <c r="C58" s="45"/>
       <c r="D58" s="131"/>
@@ -9182,7 +9185,7 @@
       <c r="AI58" s="56"/>
     </row>
     <row r="59" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A59" s="192"/>
+      <c r="A59" s="195"/>
       <c r="B59" s="57"/>
       <c r="C59" s="59"/>
       <c r="D59" s="58"/>
@@ -9211,7 +9214,7 @@
       <c r="AI59" s="62"/>
     </row>
     <row r="60" spans="1:35">
-      <c r="A60" s="200" t="s">
+      <c r="A60" s="190" t="s">
         <v>174</v>
       </c>
       <c r="B60" s="38">
@@ -9299,7 +9302,7 @@
       </c>
     </row>
     <row r="61" spans="1:35">
-      <c r="A61" s="201"/>
+      <c r="A61" s="191"/>
       <c r="B61" s="41">
         <f>B60</f>
         <v>44732</v>
@@ -9409,7 +9412,7 @@
       </c>
     </row>
     <row r="62" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A62" s="201"/>
+      <c r="A62" s="191"/>
       <c r="B62" s="44" t="s">
         <v>338</v>
       </c>
@@ -9493,7 +9496,7 @@
       </c>
     </row>
     <row r="63" spans="1:35">
-      <c r="A63" s="201"/>
+      <c r="A63" s="191"/>
       <c r="B63" s="54"/>
       <c r="H63" s="56"/>
       <c r="I63" s="39">
@@ -9516,7 +9519,7 @@
       <c r="AI63" s="56"/>
     </row>
     <row r="64" spans="1:35">
-      <c r="A64" s="201"/>
+      <c r="A64" s="191"/>
       <c r="B64" s="54"/>
       <c r="E64" s="45"/>
       <c r="H64" s="56"/>
@@ -9544,7 +9547,7 @@
       <c r="AI64" s="56"/>
     </row>
     <row r="65" spans="1:35">
-      <c r="A65" s="201"/>
+      <c r="A65" s="191"/>
       <c r="B65" s="54"/>
       <c r="E65" s="45"/>
       <c r="H65" s="56"/>
@@ -9568,7 +9571,7 @@
       <c r="AI65" s="56"/>
     </row>
     <row r="66" spans="1:35">
-      <c r="A66" s="201"/>
+      <c r="A66" s="191"/>
       <c r="B66" s="54"/>
       <c r="E66" s="45"/>
       <c r="H66" s="56"/>
@@ -9579,7 +9582,7 @@
       <c r="AI66" s="56"/>
     </row>
     <row r="67" spans="1:35">
-      <c r="A67" s="201"/>
+      <c r="A67" s="191"/>
       <c r="B67" s="54"/>
       <c r="E67" s="45"/>
       <c r="H67" s="56"/>
@@ -9589,7 +9592,7 @@
       <c r="AI67" s="56"/>
     </row>
     <row r="68" spans="1:35">
-      <c r="A68" s="201"/>
+      <c r="A68" s="191"/>
       <c r="B68" s="54"/>
       <c r="E68" s="45"/>
       <c r="H68" s="56"/>
@@ -9599,7 +9602,7 @@
       <c r="AI68" s="56"/>
     </row>
     <row r="69" spans="1:35">
-      <c r="A69" s="201"/>
+      <c r="A69" s="191"/>
       <c r="B69" s="54"/>
       <c r="E69" s="45"/>
       <c r="H69" s="56"/>
@@ -9609,7 +9612,7 @@
       <c r="AI69" s="56"/>
     </row>
     <row r="70" spans="1:35">
-      <c r="A70" s="201"/>
+      <c r="A70" s="191"/>
       <c r="B70" s="54"/>
       <c r="E70" s="45"/>
       <c r="H70" s="56"/>
@@ -9619,7 +9622,7 @@
       <c r="AI70" s="56"/>
     </row>
     <row r="71" spans="1:35">
-      <c r="A71" s="201"/>
+      <c r="A71" s="191"/>
       <c r="B71" s="54"/>
       <c r="E71" s="45"/>
       <c r="H71" s="56"/>
@@ -9629,7 +9632,7 @@
       <c r="AI71" s="56"/>
     </row>
     <row r="72" spans="1:35">
-      <c r="A72" s="201"/>
+      <c r="A72" s="191"/>
       <c r="B72" s="54"/>
       <c r="E72" s="45"/>
       <c r="H72" s="56"/>
@@ -9639,7 +9642,7 @@
       <c r="AI72" s="56"/>
     </row>
     <row r="73" spans="1:35">
-      <c r="A73" s="201"/>
+      <c r="A73" s="191"/>
       <c r="B73" s="54"/>
       <c r="E73" s="45"/>
       <c r="H73" s="56"/>
@@ -9649,7 +9652,7 @@
       <c r="AI73" s="56"/>
     </row>
     <row r="74" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A74" s="202"/>
+      <c r="A74" s="192"/>
       <c r="B74" s="54"/>
       <c r="C74" s="59"/>
       <c r="D74" s="59"/>
@@ -9685,7 +9688,7 @@
       <c r="AI74" s="62"/>
     </row>
     <row r="75" spans="1:35">
-      <c r="A75" s="190" t="s">
+      <c r="A75" s="193" t="s">
         <v>182</v>
       </c>
       <c r="B75" s="38">
@@ -9746,7 +9749,7 @@
       <c r="AI75" s="75"/>
     </row>
     <row r="76" spans="1:35">
-      <c r="A76" s="191"/>
+      <c r="A76" s="194"/>
       <c r="B76" s="41">
         <f>B75</f>
         <v>44746</v>
@@ -9799,7 +9802,7 @@
       <c r="AI76" s="56"/>
     </row>
     <row r="77" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A77" s="191"/>
+      <c r="A77" s="194"/>
       <c r="B77" s="44" t="s">
         <v>31</v>
       </c>
@@ -9841,7 +9844,7 @@
       <c r="AI77" s="56"/>
     </row>
     <row r="78" spans="1:35">
-      <c r="A78" s="191"/>
+      <c r="A78" s="194"/>
       <c r="B78" s="54"/>
       <c r="E78" s="45"/>
       <c r="H78" s="56"/>
@@ -9851,7 +9854,7 @@
       <c r="AI78" s="56"/>
     </row>
     <row r="79" spans="1:35">
-      <c r="A79" s="191"/>
+      <c r="A79" s="194"/>
       <c r="B79" s="54"/>
       <c r="E79" s="45"/>
       <c r="H79" s="56"/>
@@ -9861,7 +9864,7 @@
       <c r="AI79" s="56"/>
     </row>
     <row r="80" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A80" s="192"/>
+      <c r="A80" s="195"/>
       <c r="B80" s="57"/>
       <c r="C80" s="59"/>
       <c r="D80" s="59"/>
@@ -9893,7 +9896,7 @@
       <c r="AI80" s="62"/>
     </row>
     <row r="81" spans="1:35">
-      <c r="A81" s="200" t="s">
+      <c r="A81" s="190" t="s">
         <v>186</v>
       </c>
       <c r="B81" s="54"/>
@@ -9963,7 +9966,7 @@
       <c r="AI81" s="75"/>
     </row>
     <row r="82" spans="1:35">
-      <c r="A82" s="201"/>
+      <c r="A82" s="191"/>
       <c r="B82" s="54"/>
       <c r="D82" s="41">
         <f>D81</f>
@@ -10034,7 +10037,7 @@
       <c r="AI82" s="56"/>
     </row>
     <row r="83" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A83" s="201"/>
+      <c r="A83" s="191"/>
       <c r="B83" s="54"/>
       <c r="D83" s="44" t="s">
         <v>248</v>
@@ -10089,7 +10092,7 @@
       <c r="AI83" s="56"/>
     </row>
     <row r="84" spans="1:35">
-      <c r="A84" s="201"/>
+      <c r="A84" s="191"/>
       <c r="B84" s="54"/>
       <c r="D84" s="38">
         <v>44788</v>
@@ -10112,7 +10115,7 @@
       <c r="AI84" s="56"/>
     </row>
     <row r="85" spans="1:35">
-      <c r="A85" s="201"/>
+      <c r="A85" s="191"/>
       <c r="B85" s="54"/>
       <c r="D85" s="41">
         <f>D84</f>
@@ -10138,7 +10141,7 @@
       <c r="AI85" s="56"/>
     </row>
     <row r="86" spans="1:35" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A86" s="201"/>
+      <c r="A86" s="191"/>
       <c r="B86" s="54"/>
       <c r="D86" s="44" t="s">
         <v>247</v>
@@ -10161,7 +10164,7 @@
       <c r="AI86" s="56"/>
     </row>
     <row r="87" spans="1:35">
-      <c r="A87" s="201"/>
+      <c r="A87" s="191"/>
       <c r="B87" s="54"/>
       <c r="E87" s="45"/>
       <c r="H87" s="56"/>
@@ -10171,7 +10174,7 @@
       <c r="AI87" s="56"/>
     </row>
     <row r="88" spans="1:35">
-      <c r="A88" s="201"/>
+      <c r="A88" s="191"/>
       <c r="B88" s="54"/>
       <c r="E88" s="45"/>
       <c r="H88" s="56"/>
@@ -10181,7 +10184,7 @@
       <c r="AI88" s="56"/>
     </row>
     <row r="89" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A89" s="202"/>
+      <c r="A89" s="192"/>
       <c r="B89" s="54"/>
       <c r="C89" s="59"/>
       <c r="D89" s="45"/>
@@ -10212,7 +10215,7 @@
       <c r="AI89" s="62"/>
     </row>
     <row r="90" spans="1:35">
-      <c r="A90" s="190" t="s">
+      <c r="A90" s="193" t="s">
         <v>196</v>
       </c>
       <c r="B90" s="38">
@@ -10273,7 +10276,7 @@
       <c r="AI90" s="75"/>
     </row>
     <row r="91" spans="1:35">
-      <c r="A91" s="191"/>
+      <c r="A91" s="194"/>
       <c r="B91" s="41">
         <f t="shared" ref="B91:H91" si="64">B90</f>
         <v>44809</v>
@@ -10329,7 +10332,7 @@
       <c r="AI91" s="56"/>
     </row>
     <row r="92" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A92" s="191"/>
+      <c r="A92" s="194"/>
       <c r="B92" s="43" t="s">
         <v>151</v>
       </c>
@@ -10375,7 +10378,7 @@
       <c r="AI92" s="56"/>
     </row>
     <row r="93" spans="1:35">
-      <c r="A93" s="191"/>
+      <c r="A93" s="194"/>
       <c r="B93" s="54"/>
       <c r="E93" s="45"/>
       <c r="H93" s="56"/>
@@ -10388,7 +10391,7 @@
       <c r="AI93" s="56"/>
     </row>
     <row r="94" spans="1:35">
-      <c r="A94" s="191"/>
+      <c r="A94" s="194"/>
       <c r="B94" s="54"/>
       <c r="E94" s="45"/>
       <c r="H94" s="56"/>
@@ -10402,7 +10405,7 @@
       <c r="AI94" s="56"/>
     </row>
     <row r="95" spans="1:35">
-      <c r="A95" s="191"/>
+      <c r="A95" s="194"/>
       <c r="B95" s="54"/>
       <c r="E95" s="45"/>
       <c r="H95" s="56"/>
@@ -10415,7 +10418,7 @@
       <c r="AI95" s="56"/>
     </row>
     <row r="96" spans="1:35">
-      <c r="A96" s="191"/>
+      <c r="A96" s="194"/>
       <c r="B96" s="54"/>
       <c r="E96" s="45"/>
       <c r="H96" s="56"/>
@@ -10425,7 +10428,7 @@
       <c r="AI96" s="56"/>
     </row>
     <row r="97" spans="1:35">
-      <c r="A97" s="191"/>
+      <c r="A97" s="194"/>
       <c r="B97" s="54"/>
       <c r="E97" s="45"/>
       <c r="H97" s="56"/>
@@ -10435,7 +10438,7 @@
       <c r="AI97" s="56"/>
     </row>
     <row r="98" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A98" s="192"/>
+      <c r="A98" s="195"/>
       <c r="B98" s="54"/>
       <c r="C98" s="59"/>
       <c r="D98" s="59"/>
@@ -10470,7 +10473,7 @@
       <c r="AI98" s="62"/>
     </row>
     <row r="99" spans="1:35">
-      <c r="A99" s="200" t="s">
+      <c r="A99" s="190" t="s">
         <v>199</v>
       </c>
       <c r="E99" s="63">
@@ -10542,7 +10545,7 @@
       </c>
     </row>
     <row r="100" spans="1:35">
-      <c r="A100" s="201"/>
+      <c r="A100" s="191"/>
       <c r="E100" s="65">
         <f>E99</f>
         <v>44844</v>
@@ -10625,7 +10628,7 @@
       </c>
     </row>
     <row r="101" spans="1:35" ht="39" thickBot="1">
-      <c r="A101" s="201"/>
+      <c r="A101" s="191"/>
       <c r="E101" s="67" t="s">
         <v>200</v>
       </c>
@@ -10689,7 +10692,7 @@
       </c>
     </row>
     <row r="102" spans="1:35">
-      <c r="A102" s="201"/>
+      <c r="A102" s="191"/>
       <c r="E102" s="113"/>
       <c r="G102" s="87"/>
       <c r="H102" s="104"/>
@@ -10709,7 +10712,7 @@
       <c r="AI102" s="104"/>
     </row>
     <row r="103" spans="1:35">
-      <c r="A103" s="201"/>
+      <c r="A103" s="191"/>
       <c r="E103" s="113"/>
       <c r="G103" s="87"/>
       <c r="H103" s="104"/>
@@ -10729,7 +10732,7 @@
       <c r="AI103" s="104"/>
     </row>
     <row r="104" spans="1:35">
-      <c r="A104" s="201"/>
+      <c r="A104" s="191"/>
       <c r="E104" s="113"/>
       <c r="G104" s="87"/>
       <c r="H104" s="104"/>
@@ -10749,7 +10752,7 @@
       <c r="AI104" s="104"/>
     </row>
     <row r="105" spans="1:35">
-      <c r="A105" s="201"/>
+      <c r="A105" s="191"/>
       <c r="E105" s="113"/>
       <c r="G105" s="87"/>
       <c r="H105" s="56"/>
@@ -10769,7 +10772,7 @@
       <c r="AI105" s="104"/>
     </row>
     <row r="106" spans="1:35">
-      <c r="A106" s="201"/>
+      <c r="A106" s="191"/>
       <c r="E106" s="113"/>
       <c r="G106" s="87"/>
       <c r="H106" s="56"/>
@@ -10789,7 +10792,7 @@
       <c r="AI106" s="104"/>
     </row>
     <row r="107" spans="1:35">
-      <c r="A107" s="201"/>
+      <c r="A107" s="191"/>
       <c r="E107" s="113"/>
       <c r="G107" s="87"/>
       <c r="H107" s="104"/>
@@ -10809,7 +10812,7 @@
       <c r="AI107" s="104"/>
     </row>
     <row r="108" spans="1:35">
-      <c r="A108" s="201"/>
+      <c r="A108" s="191"/>
       <c r="E108" s="45"/>
       <c r="H108" s="56"/>
       <c r="P108" s="29"/>
@@ -10818,7 +10821,7 @@
       <c r="AI108" s="56"/>
     </row>
     <row r="109" spans="1:35">
-      <c r="A109" s="201"/>
+      <c r="A109" s="191"/>
       <c r="E109" s="45"/>
       <c r="H109" s="56"/>
       <c r="P109" s="29"/>
@@ -10827,7 +10830,7 @@
       <c r="AI109" s="56"/>
     </row>
     <row r="110" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A110" s="202"/>
+      <c r="A110" s="192"/>
       <c r="B110" s="58"/>
       <c r="C110" s="59"/>
       <c r="D110" s="59"/>
@@ -10861,7 +10864,7 @@
       <c r="AI110" s="62"/>
     </row>
     <row r="111" spans="1:35">
-      <c r="A111" s="190" t="s">
+      <c r="A111" s="193" t="s">
         <v>204</v>
       </c>
       <c r="B111" s="38">
@@ -10924,7 +10927,7 @@
       </c>
     </row>
     <row r="112" spans="1:35">
-      <c r="A112" s="191"/>
+      <c r="A112" s="194"/>
       <c r="B112" s="41">
         <f>B111</f>
         <v>44876</v>
@@ -10986,7 +10989,7 @@
       </c>
     </row>
     <row r="113" spans="1:35" ht="51.75" thickBot="1">
-      <c r="A113" s="191"/>
+      <c r="A113" s="194"/>
       <c r="B113" s="44" t="s">
         <v>329</v>
       </c>
@@ -11034,7 +11037,7 @@
       </c>
     </row>
     <row r="114" spans="1:35">
-      <c r="A114" s="191"/>
+      <c r="A114" s="194"/>
       <c r="B114" s="38">
         <v>44889</v>
       </c>
@@ -11059,7 +11062,7 @@
       <c r="AI114" s="56"/>
     </row>
     <row r="115" spans="1:35">
-      <c r="A115" s="191"/>
+      <c r="A115" s="194"/>
       <c r="B115" s="41">
         <f>B114</f>
         <v>44889</v>
@@ -11087,7 +11090,7 @@
       <c r="AI115" s="56"/>
     </row>
     <row r="116" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A116" s="191"/>
+      <c r="A116" s="194"/>
       <c r="B116" s="44" t="s">
         <v>238</v>
       </c>
@@ -11110,7 +11113,7 @@
       <c r="AI116" s="56"/>
     </row>
     <row r="117" spans="1:35">
-      <c r="A117" s="191"/>
+      <c r="A117" s="194"/>
       <c r="B117" s="38">
         <v>44890</v>
       </c>
@@ -11122,7 +11125,7 @@
       <c r="AI117" s="56"/>
     </row>
     <row r="118" spans="1:35">
-      <c r="A118" s="191"/>
+      <c r="A118" s="194"/>
       <c r="B118" s="41">
         <f>B117</f>
         <v>44890</v>
@@ -11135,7 +11138,7 @@
       <c r="AI118" s="56"/>
     </row>
     <row r="119" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A119" s="191"/>
+      <c r="A119" s="194"/>
       <c r="B119" s="44" t="s">
         <v>334</v>
       </c>
@@ -11147,7 +11150,7 @@
       <c r="AI119" s="56"/>
     </row>
     <row r="120" spans="1:35">
-      <c r="A120" s="191"/>
+      <c r="A120" s="194"/>
       <c r="B120" s="45"/>
       <c r="E120" s="45"/>
       <c r="H120" s="56"/>
@@ -11157,7 +11160,7 @@
       <c r="AI120" s="56"/>
     </row>
     <row r="121" spans="1:35">
-      <c r="A121" s="191"/>
+      <c r="A121" s="194"/>
       <c r="B121" s="54"/>
       <c r="E121" s="45"/>
       <c r="H121" s="56"/>
@@ -11167,7 +11170,7 @@
       <c r="AI121" s="56"/>
     </row>
     <row r="122" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A122" s="192"/>
+      <c r="A122" s="195"/>
       <c r="B122" s="54"/>
       <c r="D122" s="62"/>
       <c r="E122" s="59"/>
@@ -11197,7 +11200,7 @@
       <c r="AI122" s="58"/>
     </row>
     <row r="123" spans="1:35">
-      <c r="A123" s="200" t="s">
+      <c r="A123" s="190" t="s">
         <v>214</v>
       </c>
       <c r="B123" s="37">
@@ -11296,7 +11299,7 @@
       </c>
     </row>
     <row r="124" spans="1:35">
-      <c r="A124" s="201"/>
+      <c r="A124" s="191"/>
       <c r="B124" s="40">
         <f t="shared" ref="B124" si="66">B123</f>
         <v>44921</v>
@@ -11419,7 +11422,7 @@
       </c>
     </row>
     <row r="125" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A125" s="201"/>
+      <c r="A125" s="191"/>
       <c r="B125" s="43" t="s">
         <v>215</v>
       </c>
@@ -11512,7 +11515,7 @@
       </c>
     </row>
     <row r="126" spans="1:35">
-      <c r="A126" s="201"/>
+      <c r="A126" s="191"/>
       <c r="B126" s="54"/>
       <c r="D126" s="63">
         <v>44921</v>
@@ -11576,7 +11579,7 @@
       </c>
     </row>
     <row r="127" spans="1:35">
-      <c r="A127" s="201"/>
+      <c r="A127" s="191"/>
       <c r="B127" s="54"/>
       <c r="D127" s="65">
         <f t="shared" ref="D127" si="76">D126</f>
@@ -11659,7 +11662,7 @@
       </c>
     </row>
     <row r="128" spans="1:35" ht="26.25" thickBot="1">
-      <c r="A128" s="201"/>
+      <c r="A128" s="191"/>
       <c r="B128" s="54"/>
       <c r="D128" s="119" t="s">
         <v>215</v>
@@ -11723,7 +11726,7 @@
       </c>
     </row>
     <row r="129" spans="1:35">
-      <c r="A129" s="201"/>
+      <c r="A129" s="191"/>
       <c r="B129" s="54"/>
       <c r="E129" s="45"/>
       <c r="G129" s="120"/>
@@ -11734,7 +11737,7 @@
       <c r="AI129" s="56"/>
     </row>
     <row r="130" spans="1:35">
-      <c r="A130" s="201"/>
+      <c r="A130" s="191"/>
       <c r="B130" s="54"/>
       <c r="E130" s="45"/>
       <c r="G130" s="120"/>
@@ -11745,7 +11748,7 @@
       <c r="AI130" s="56"/>
     </row>
     <row r="131" spans="1:35">
-      <c r="A131" s="201"/>
+      <c r="A131" s="191"/>
       <c r="B131" s="54"/>
       <c r="E131" s="45"/>
       <c r="G131" s="120"/>
@@ -11756,7 +11759,7 @@
       <c r="AI131" s="56"/>
     </row>
     <row r="132" spans="1:35">
-      <c r="A132" s="201"/>
+      <c r="A132" s="191"/>
       <c r="B132" s="54"/>
       <c r="E132" s="45"/>
       <c r="H132" s="56"/>
@@ -11766,7 +11769,7 @@
       <c r="AI132" s="56"/>
     </row>
     <row r="133" spans="1:35">
-      <c r="A133" s="201"/>
+      <c r="A133" s="191"/>
       <c r="B133" s="54"/>
       <c r="E133" s="45"/>
       <c r="H133" s="56"/>
@@ -11776,7 +11779,7 @@
       <c r="AI133" s="56"/>
     </row>
     <row r="134" spans="1:35" ht="15.75" thickBot="1">
-      <c r="A134" s="202"/>
+      <c r="A134" s="192"/>
       <c r="B134" s="57"/>
       <c r="C134" s="59"/>
       <c r="D134" s="59"/>
@@ -13258,6 +13261,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A15:A20"/>
     <mergeCell ref="A99:A110"/>
     <mergeCell ref="A111:A122"/>
     <mergeCell ref="A123:A134"/>
@@ -13267,12 +13276,6 @@
     <mergeCell ref="A75:A80"/>
     <mergeCell ref="A81:A89"/>
     <mergeCell ref="A90:A98"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Z1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="A3:A14"/>
-    <mergeCell ref="A15:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13295,7 +13298,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="207" t="s">
         <v>236</v>
       </c>
       <c r="B1" s="135" t="s">
@@ -13303,27 +13306,27 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="219"/>
+      <c r="A2" s="207"/>
       <c r="B2" s="136" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="219"/>
+      <c r="A3" s="207"/>
       <c r="B3" s="137"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="219"/>
+      <c r="A4" s="207"/>
       <c r="B4" s="137"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="220"/>
+      <c r="A5" s="208"/>
       <c r="B5" s="138">
         <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="221" t="s">
+      <c r="A6" s="209" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="38">
@@ -13331,50 +13334,50 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="222"/>
+      <c r="A7" s="210"/>
       <c r="B7" s="41">
         <f t="shared" ref="B7" si="0">B6</f>
         <v>44564</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A8" s="222"/>
+      <c r="A8" s="210"/>
       <c r="B8" s="43" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="223" t="s">
+      <c r="A9" s="211" t="s">
         <v>137</v>
       </c>
       <c r="B9" s="141"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="223"/>
+      <c r="A10" s="211"/>
       <c r="B10" s="142"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="224" t="s">
+      <c r="A11" s="212" t="s">
         <v>148</v>
       </c>
       <c r="B11" s="139"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="224"/>
+      <c r="A12" s="212"/>
       <c r="B12" s="140"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="225" t="s">
+      <c r="A13" s="213" t="s">
         <v>154</v>
       </c>
       <c r="B13" s="141"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A14" s="225"/>
+      <c r="A14" s="213"/>
       <c r="B14" s="142"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="216" t="s">
+      <c r="A15" s="205" t="s">
         <v>159</v>
       </c>
       <c r="B15" s="88">
@@ -13382,20 +13385,20 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="216"/>
+      <c r="A16" s="205"/>
       <c r="B16" s="90">
         <f>B15</f>
         <v>44711</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A17" s="218"/>
+      <c r="A17" s="206"/>
       <c r="B17" s="92" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="206" t="s">
+      <c r="A18" s="215" t="s">
         <v>174</v>
       </c>
       <c r="B18" s="167">
@@ -13403,20 +13406,20 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="207"/>
+      <c r="A19" s="216"/>
       <c r="B19" s="168">
         <f>B18</f>
         <v>44732</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.25" thickBot="1">
-      <c r="A20" s="208"/>
+      <c r="A20" s="217"/>
       <c r="B20" s="166" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="209" t="s">
+      <c r="A21" s="218" t="s">
         <v>182</v>
       </c>
       <c r="B21" s="38">
@@ -13424,30 +13427,30 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="210"/>
+      <c r="A22" s="219"/>
       <c r="B22" s="41">
         <f>B21</f>
         <v>44746</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A23" s="210"/>
+      <c r="A23" s="219"/>
       <c r="B23" s="44" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="220" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="213"/>
+      <c r="B24" s="222"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A25" s="212"/>
-      <c r="B25" s="214"/>
+      <c r="A25" s="221"/>
+      <c r="B25" s="223"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="215" t="s">
+      <c r="A26" s="224" t="s">
         <v>196</v>
       </c>
       <c r="B26" s="38">
@@ -13455,30 +13458,30 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="216"/>
+      <c r="A27" s="205"/>
       <c r="B27" s="41">
         <f t="shared" ref="B27" si="1">B26</f>
         <v>44809</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A28" s="216"/>
+      <c r="A28" s="205"/>
       <c r="B28" s="43" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="217" t="s">
+      <c r="A29" s="225" t="s">
         <v>199</v>
       </c>
       <c r="B29" s="143"/>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A30" s="211"/>
+      <c r="A30" s="220"/>
       <c r="B30" s="143"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="205" t="s">
+      <c r="A31" s="214" t="s">
         <v>204</v>
       </c>
       <c r="B31" s="37">
@@ -13486,39 +13489,39 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="205"/>
+      <c r="A32" s="214"/>
       <c r="B32" s="144">
         <f>B31</f>
         <v>44876</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="51.75" thickBot="1">
-      <c r="A33" s="205"/>
+      <c r="A33" s="214"/>
       <c r="B33" s="145" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="205"/>
+      <c r="A34" s="214"/>
       <c r="B34" s="38">
         <v>44889</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="205"/>
+      <c r="A35" s="214"/>
       <c r="B35" s="41">
         <f>B34</f>
         <v>44889</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A36" s="205"/>
+      <c r="A36" s="214"/>
       <c r="B36" s="44" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A37" s="205"/>
+      <c r="A37" s="214"/>
       <c r="B37" s="147"/>
     </row>
     <row r="38" spans="1:2">
@@ -13552,12 +13555,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A31:A37"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
@@ -13565,6 +13562,12 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13587,7 +13590,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="207" t="s">
         <v>236</v>
       </c>
       <c r="B1" s="135" t="s">
@@ -13595,27 +13598,27 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="219"/>
+      <c r="A2" s="207"/>
       <c r="B2" s="136" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="219"/>
+      <c r="A3" s="207"/>
       <c r="B3" s="137"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="219"/>
+      <c r="A4" s="207"/>
       <c r="B4" s="137"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="220"/>
+      <c r="A5" s="208"/>
       <c r="B5" s="138">
         <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="221" t="s">
+      <c r="A6" s="209" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="38">
@@ -13623,50 +13626,50 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="222"/>
+      <c r="A7" s="210"/>
       <c r="B7" s="41">
         <f t="shared" ref="B7" si="0">B6</f>
         <v>44564</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A8" s="222"/>
+      <c r="A8" s="210"/>
       <c r="B8" s="43" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="223" t="s">
+      <c r="A9" s="211" t="s">
         <v>137</v>
       </c>
       <c r="B9" s="141"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="223"/>
+      <c r="A10" s="211"/>
       <c r="B10" s="142"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="224" t="s">
+      <c r="A11" s="212" t="s">
         <v>148</v>
       </c>
       <c r="B11" s="139"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="224"/>
+      <c r="A12" s="212"/>
       <c r="B12" s="140"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="225" t="s">
+      <c r="A13" s="213" t="s">
         <v>154</v>
       </c>
       <c r="B13" s="141"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A14" s="225"/>
+      <c r="A14" s="213"/>
       <c r="B14" s="142"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="216" t="s">
+      <c r="A15" s="205" t="s">
         <v>159</v>
       </c>
       <c r="B15" s="88">
@@ -13674,20 +13677,20 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="216"/>
+      <c r="A16" s="205"/>
       <c r="B16" s="90">
         <f>B15</f>
         <v>44711</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A17" s="218"/>
+      <c r="A17" s="206"/>
       <c r="B17" s="92" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="225" t="s">
+      <c r="A18" s="213" t="s">
         <v>174</v>
       </c>
       <c r="B18" s="167">
@@ -13695,20 +13698,20 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="225"/>
+      <c r="A19" s="213"/>
       <c r="B19" s="168">
         <f>B18</f>
         <v>44732</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.25" thickBot="1">
-      <c r="A20" s="225"/>
+      <c r="A20" s="213"/>
       <c r="B20" s="166" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="224" t="s">
         <v>182</v>
       </c>
       <c r="B21" s="38">
@@ -13716,30 +13719,30 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="216"/>
+      <c r="A22" s="205"/>
       <c r="B22" s="41">
         <f>B21</f>
         <v>44746</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A23" s="216"/>
+      <c r="A23" s="205"/>
       <c r="B23" s="44" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="220" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="213"/>
+      <c r="B24" s="222"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A25" s="212"/>
-      <c r="B25" s="214"/>
+      <c r="A25" s="221"/>
+      <c r="B25" s="223"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="215" t="s">
+      <c r="A26" s="224" t="s">
         <v>196</v>
       </c>
       <c r="B26" s="38">
@@ -13747,30 +13750,30 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="216"/>
+      <c r="A27" s="205"/>
       <c r="B27" s="41">
         <f t="shared" ref="B27" si="1">B26</f>
         <v>44809</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A28" s="216"/>
+      <c r="A28" s="205"/>
       <c r="B28" s="43" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="217" t="s">
+      <c r="A29" s="225" t="s">
         <v>199</v>
       </c>
       <c r="B29" s="143"/>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A30" s="211"/>
+      <c r="A30" s="220"/>
       <c r="B30" s="143"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="205" t="s">
+      <c r="A31" s="214" t="s">
         <v>204</v>
       </c>
       <c r="B31" s="37">
@@ -13778,39 +13781,39 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="205"/>
+      <c r="A32" s="214"/>
       <c r="B32" s="144">
         <f>B31</f>
         <v>44876</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="64.5" thickBot="1">
-      <c r="A33" s="205"/>
+      <c r="A33" s="214"/>
       <c r="B33" s="145" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="205"/>
+      <c r="A34" s="214"/>
       <c r="B34" s="38">
         <v>44889</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="205"/>
+      <c r="A35" s="214"/>
       <c r="B35" s="41">
         <f>B34</f>
         <v>44889</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A36" s="205"/>
+      <c r="A36" s="214"/>
       <c r="B36" s="44" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A37" s="205"/>
+      <c r="A37" s="214"/>
       <c r="B37" s="147"/>
     </row>
     <row r="38" spans="1:2">
@@ -13844,12 +13847,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A31:A37"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
@@ -13857,6 +13854,12 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13878,7 +13881,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="228" t="s">
         <v>236</v>
       </c>
       <c r="B1" s="152" t="s">
@@ -13886,54 +13889,54 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="235"/>
+      <c r="A2" s="229"/>
       <c r="B2" s="153" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="235"/>
+      <c r="A3" s="229"/>
       <c r="B3" s="154"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="235"/>
+      <c r="A4" s="229"/>
       <c r="B4" s="154"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="236"/>
+      <c r="A5" s="230"/>
       <c r="B5" s="155">
         <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="228" t="s">
+      <c r="A6" s="231" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="38"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="229"/>
+      <c r="A7" s="226"/>
       <c r="B7" s="41"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A8" s="229"/>
+      <c r="A8" s="226"/>
       <c r="B8" s="43"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="229"/>
+      <c r="A9" s="226"/>
       <c r="B9" s="37">
         <v>44578</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="229"/>
+      <c r="A10" s="226"/>
       <c r="B10" s="40">
         <f>B9</f>
         <v>44578</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A11" s="229"/>
+      <c r="A11" s="226"/>
       <c r="B11" s="43" t="s">
         <v>130</v>
       </c>
@@ -13945,7 +13948,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="237" t="s">
+      <c r="A13" s="232" t="s">
         <v>137</v>
       </c>
       <c r="B13" s="174">
@@ -13954,19 +13957,19 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="237"/>
+      <c r="A14" s="232"/>
       <c r="B14" s="175" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="238" t="s">
+      <c r="A15" s="233" t="s">
         <v>148</v>
       </c>
       <c r="B15" s="156"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="238"/>
+      <c r="A16" s="233"/>
       <c r="B16" s="157"/>
     </row>
     <row r="17" spans="1:2">
@@ -13974,17 +13977,17 @@
       <c r="B17" s="171"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="227" t="s">
+      <c r="A18" s="234" t="s">
         <v>154</v>
       </c>
       <c r="B18" s="158"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A19" s="227"/>
+      <c r="A19" s="234"/>
       <c r="B19" s="159"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="229" t="s">
+      <c r="A20" s="226" t="s">
         <v>159</v>
       </c>
       <c r="B20" s="88">
@@ -13992,34 +13995,34 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="229"/>
+      <c r="A21" s="226"/>
       <c r="B21" s="90">
         <f>B20</f>
         <v>44711</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A22" s="233"/>
+      <c r="A22" s="227"/>
       <c r="B22" s="92" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="227" t="s">
+      <c r="A23" s="234" t="s">
         <v>174</v>
       </c>
       <c r="B23" s="167"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="227"/>
+      <c r="A24" s="234"/>
       <c r="B24" s="168"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A25" s="227"/>
+      <c r="A25" s="234"/>
       <c r="B25" s="166"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="228" t="s">
+      <c r="A26" s="231" t="s">
         <v>182</v>
       </c>
       <c r="B26" s="38">
@@ -14027,30 +14030,30 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="229"/>
+      <c r="A27" s="226"/>
       <c r="B27" s="41">
         <f>B26</f>
         <v>44746</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A28" s="229"/>
+      <c r="A28" s="226"/>
       <c r="B28" s="44" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="230" t="s">
+      <c r="A29" s="236" t="s">
         <v>186</v>
       </c>
       <c r="B29" s="158"/>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A30" s="230"/>
+      <c r="A30" s="236"/>
       <c r="B30" s="159"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="228" t="s">
+      <c r="A31" s="231" t="s">
         <v>196</v>
       </c>
       <c r="B31" s="38">
@@ -14058,30 +14061,30 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="229"/>
+      <c r="A32" s="226"/>
       <c r="B32" s="41">
         <f t="shared" ref="B32" si="0">B31</f>
         <v>44809</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A33" s="229"/>
+      <c r="A33" s="226"/>
       <c r="B33" s="43" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="231" t="s">
+      <c r="A34" s="237" t="s">
         <v>199</v>
       </c>
       <c r="B34" s="160"/>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A35" s="232"/>
+      <c r="A35" s="238"/>
       <c r="B35" s="160"/>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="205" t="s">
+      <c r="A36" s="214" t="s">
         <v>204</v>
       </c>
       <c r="B36" s="38">
@@ -14089,20 +14092,20 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="205"/>
+      <c r="A37" s="214"/>
       <c r="B37" s="41">
         <f>B36</f>
         <v>44889</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A38" s="205"/>
+      <c r="A38" s="214"/>
       <c r="B38" s="44" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="226" t="s">
+      <c r="A39" s="235" t="s">
         <v>214</v>
       </c>
       <c r="B39" s="37">
@@ -14110,14 +14113,14 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="223"/>
+      <c r="A40" s="211"/>
       <c r="B40" s="40">
         <f t="shared" ref="B40" si="1">B39</f>
         <v>44921</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A41" s="223"/>
+      <c r="A41" s="211"/>
       <c r="B41" s="43" t="s">
         <v>215</v>
       </c>
@@ -14132,12 +14135,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:A19"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A28"/>
@@ -14145,6 +14142,12 @@
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14166,7 +14169,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="207" t="s">
         <v>236</v>
       </c>
       <c r="B1" s="135" t="s">
@@ -14174,27 +14177,27 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="219"/>
+      <c r="A2" s="207"/>
       <c r="B2" s="136" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="219"/>
+      <c r="A3" s="207"/>
       <c r="B3" s="137"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="219"/>
+      <c r="A4" s="207"/>
       <c r="B4" s="137"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="220"/>
+      <c r="A5" s="208"/>
       <c r="B5" s="138">
         <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="221" t="s">
+      <c r="A6" s="209" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="38">
@@ -14202,50 +14205,50 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="222"/>
+      <c r="A7" s="210"/>
       <c r="B7" s="41">
         <f t="shared" ref="B7" si="0">B6</f>
         <v>44564</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A8" s="222"/>
+      <c r="A8" s="210"/>
       <c r="B8" s="43" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="223" t="s">
+      <c r="A9" s="211" t="s">
         <v>137</v>
       </c>
       <c r="B9" s="141"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="223"/>
+      <c r="A10" s="211"/>
       <c r="B10" s="142"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="224" t="s">
+      <c r="A11" s="212" t="s">
         <v>148</v>
       </c>
       <c r="B11" s="139"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="224"/>
+      <c r="A12" s="212"/>
       <c r="B12" s="140"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="225" t="s">
+      <c r="A13" s="213" t="s">
         <v>154</v>
       </c>
       <c r="B13" s="141"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A14" s="225"/>
+      <c r="A14" s="213"/>
       <c r="B14" s="142"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="216" t="s">
+      <c r="A15" s="205" t="s">
         <v>159</v>
       </c>
       <c r="B15" s="88">
@@ -14253,20 +14256,20 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="216"/>
+      <c r="A16" s="205"/>
       <c r="B16" s="90">
         <f>B15</f>
         <v>44711</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A17" s="218"/>
+      <c r="A17" s="206"/>
       <c r="B17" s="92" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="225" t="s">
+      <c r="A18" s="213" t="s">
         <v>174</v>
       </c>
       <c r="B18" s="167">
@@ -14274,20 +14277,20 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="225"/>
+      <c r="A19" s="213"/>
       <c r="B19" s="168">
         <f>B18</f>
         <v>44732</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.25" thickBot="1">
-      <c r="A20" s="225"/>
+      <c r="A20" s="213"/>
       <c r="B20" s="166" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="224" t="s">
         <v>182</v>
       </c>
       <c r="B21" s="38">
@@ -14295,30 +14298,30 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="216"/>
+      <c r="A22" s="205"/>
       <c r="B22" s="41">
         <f>B21</f>
         <v>44746</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A23" s="216"/>
+      <c r="A23" s="205"/>
       <c r="B23" s="44" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="220" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="213"/>
+      <c r="B24" s="222"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A25" s="212"/>
-      <c r="B25" s="214"/>
+      <c r="A25" s="221"/>
+      <c r="B25" s="223"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="215" t="s">
+      <c r="A26" s="224" t="s">
         <v>196</v>
       </c>
       <c r="B26" s="38">
@@ -14326,30 +14329,30 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="216"/>
+      <c r="A27" s="205"/>
       <c r="B27" s="41">
         <f t="shared" ref="B27" si="1">B26</f>
         <v>44809</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A28" s="216"/>
+      <c r="A28" s="205"/>
       <c r="B28" s="43" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="217" t="s">
+      <c r="A29" s="225" t="s">
         <v>199</v>
       </c>
       <c r="B29" s="143"/>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A30" s="211"/>
+      <c r="A30" s="220"/>
       <c r="B30" s="143"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="205" t="s">
+      <c r="A31" s="214" t="s">
         <v>204</v>
       </c>
       <c r="B31" s="38">
@@ -14357,33 +14360,33 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="205"/>
+      <c r="A32" s="214"/>
       <c r="B32" s="41">
         <f>B31</f>
         <v>44889</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A33" s="205"/>
+      <c r="A33" s="214"/>
       <c r="B33" s="44" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="205"/>
+      <c r="A34" s="214"/>
       <c r="B34" s="38">
         <v>44890</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="205"/>
+      <c r="A35" s="214"/>
       <c r="B35" s="146">
         <f>B34</f>
         <v>44890</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A36" s="205"/>
+      <c r="A36" s="214"/>
       <c r="B36" s="146" t="s">
         <v>334</v>
       </c>
@@ -14419,12 +14422,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
@@ -14432,6 +14429,12 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14443,7 +14446,7 @@
   <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14453,7 +14456,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="207" t="s">
         <v>236</v>
       </c>
       <c r="B1" s="135" t="s">
@@ -14461,21 +14464,21 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="219"/>
+      <c r="A2" s="207"/>
       <c r="B2" s="136" t="s">
-        <v>328</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="219"/>
+      <c r="A3" s="207"/>
       <c r="B3" s="137"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="219"/>
+      <c r="A4" s="207"/>
       <c r="B4" s="137"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="219"/>
+      <c r="A5" s="207"/>
       <c r="B5" s="138">
         <v>2022</v>
       </c>
@@ -14745,6 +14748,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A21:A23"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="A39:A44"/>
@@ -14753,11 +14761,6 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A21:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>